<commit_message>
finish get consequence of split port
</commit_message>
<xml_diff>
--- a/stage_modeling.xlsx
+++ b/stage_modeling.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="stage_2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="stage_5" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="stage_6" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="stage_7" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="stage_8" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -63,9 +65,24 @@
     <t xml:space="preserve">(2,2)</t>
   </si>
   <si>
+    <t xml:space="preserve">:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0,0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,0)</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1,8)</t>
   </si>
   <si>
+    <t xml:space="preserve">(2,0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3,0)</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1,13)</t>
   </si>
   <si>
@@ -87,7 +104,25 @@
     <t xml:space="preserve">(6,14)</t>
   </si>
   <si>
-    <t xml:space="preserve">(3,0)</t>
+    <t xml:space="preserve">(3,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6,3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4,9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(7,10)</t>
   </si>
 </sst>
 </file>
@@ -140,7 +175,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,7 +203,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
-        <bgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFC7A0CB"/>
       </patternFill>
     </fill>
     <fill>
@@ -199,6 +234,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
         <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7A0CB"/>
+        <bgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
   </fills>
@@ -271,7 +312,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -426,6 +467,34 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -477,7 +546,7 @@
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFF7A19A"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFC7A0CB"/>
       <rgbColor rgb="FFF8CBAD"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -505,10 +574,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -732,8 +801,26 @@
       <c r="D11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -753,8 +840,8 @@
   </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1034,10 +1121,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,15 +1132,15 @@
         <v>6</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="33" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F14" s="33"/>
       <c r="G14" s="33" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H14" s="33"/>
     </row>
@@ -1062,16 +1149,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1543,10 +1630,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1558,4 +1645,593 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+    </row>
+    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
create stage 9 + 10
</commit_message>
<xml_diff>
--- a/stage_modeling.xlsx
+++ b/stage_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="stage_2" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,8 @@
     <sheet name="stage_6" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="stage_7" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="stage_8" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="stage_9" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="stage_10" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="48">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -123,6 +125,51 @@
   </si>
   <si>
     <t xml:space="preserve">(7,10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2,12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3,12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(9,5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(9,11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4,0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5,0)</t>
   </si>
 </sst>
 </file>
@@ -312,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -494,6 +541,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1932,10 +1983,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2179,29 +2230,20 @@
       <c r="O10" s="40"/>
       <c r="P10" s="40"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -2210,20 +2252,704 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="C15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:V11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="39"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V7" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:U17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="39"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="40"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="39"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="39"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="39"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="39"/>
+    </row>
+    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="39"/>
+    </row>
+    <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="39"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U12" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="C14" s="8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="E15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
create stage 11 + refactor to write input as number
</commit_message>
<xml_diff>
--- a/stage_modeling.xlsx
+++ b/stage_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="stage_2" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="stage_8" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="stage_9" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="stage_10" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="stage_11" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="52">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -170,6 +171,18 @@
   </si>
   <si>
     <t xml:space="preserve">(5,0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0,4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6,6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0,-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,-1)</t>
   </si>
 </sst>
 </file>
@@ -359,7 +372,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -516,36 +529,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1705,14 +1714,14 @@
   </sheetPr>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="6.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1768,41 +1777,41 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1811,14 +1820,14 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -1839,9 +1848,9 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
       <c r="N5" s="3"/>
       <c r="O5" s="4" t="s">
         <v>1</v>
@@ -1855,17 +1864,17 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -1877,15 +1886,15 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -1894,41 +1903,41 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7" t="s">
@@ -1985,14 +1994,14 @@
   </sheetPr>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="6.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2048,80 +2057,80 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="43"/>
+      <c r="L3" s="41"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="44"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="44"/>
+      <c r="O5" s="42"/>
       <c r="P5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2138,9 +2147,9 @@
         <v>29</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -2160,9 +2169,9 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -2174,61 +2183,61 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7" t="s">
@@ -2295,13 +2304,13 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="6.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2361,13 +2370,13 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -2381,17 +2390,17 @@
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="43"/>
+      <c r="N3" s="41"/>
       <c r="O3" s="3" t="s">
         <v>29</v>
       </c>
@@ -2421,43 +2430,41 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="39"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="V7" s="0" t="s">
@@ -2528,14 +2535,14 @@
   </sheetPr>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="6.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="5.16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2591,11 +2598,11 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -2618,12 +2625,12 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="41" t="s">
         <v>3</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="41" t="s">
         <v>29</v>
       </c>
       <c r="O3" s="3"/>
@@ -2635,146 +2642,145 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="6"/>
-      <c r="O4" s="39"/>
+      <c r="O4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="6"/>
-      <c r="O5" s="40"/>
+      <c r="O5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="39"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="39"/>
+      <c r="O7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="39"/>
+      <c r="O8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="39"/>
+      <c r="O9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="39"/>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -2782,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="3"/>
-      <c r="O11" s="39"/>
+      <c r="O11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U12" s="0" t="s">
@@ -2960,4 +2966,353 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="14" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="44" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="44" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="44" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="44" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="45"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="45"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="45"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S12" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor class solver, node, problem to support action label for each action
</commit_message>
<xml_diff>
--- a/stage_modeling.xlsx
+++ b/stage_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="stage_2" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,10 @@
     <sheet name="stage_9" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="stage_10" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="stage_11" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="stage_12" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="stage_14" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="stage_15" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="stage_16" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="96">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -183,6 +187,138 @@
   </si>
   <si>
     <t xml:space="preserve">(1,-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6,4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2,6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0,12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,9</t>
   </si>
 </sst>
 </file>
@@ -372,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -549,12 +685,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -893,6 +1057,1404 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:U17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+    </row>
+    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+    </row>
+    <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U12" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="50" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="46"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="46"/>
+    </row>
+    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10" s="46"/>
+    </row>
+    <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="46"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V12" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="44" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="44" width="5.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="44" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="45" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="45" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="45" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="45" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="45" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="45" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="45" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="45" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="45" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="45" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="45" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="45" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="45" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="45" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="45" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+    </row>
+    <row r="10" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T10" s="51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+    </row>
+    <row r="12" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+    </row>
+    <row r="13" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+    </row>
+    <row r="14" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="52"/>
+      <c r="C14" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+    </row>
+    <row r="15" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="48"/>
+    </row>
+    <row r="16" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2535,7 +4097,7 @@
   </sheetPr>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -2975,8 +4537,12 @@
   </sheetPr>
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="Q6" activeCellId="0" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3009,19 +4575,19 @@
       <c r="H1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I1" s="44" t="n">
+      <c r="I1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J1" s="44" t="n">
+      <c r="J1" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K1" s="44" t="n">
+      <c r="K1" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="L1" s="44" t="n">
+      <c r="L1" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="M1" s="44" t="n">
+      <c r="M1" s="1" t="n">
         <v>11</v>
       </c>
     </row>
@@ -3035,11 +4601,11 @@
       <c r="F2" s="6"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -3051,12 +4617,12 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
+      <c r="G3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -3068,11 +4634,11 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -3089,7 +4655,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="45"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -3102,11 +4668,11 @@
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="45"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -3140,8 +4706,8 @@
       <c r="H8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="3"/>
@@ -3160,7 +4726,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="45"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3171,7 +4737,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="45"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -3187,15 +4753,15 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="45"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S12" s="0" t="s">
@@ -3315,4 +4881,400 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="44" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="44" width="5.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="44" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="45" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="45" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="45" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="45" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="45" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="45" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="45" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="45" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="45" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="45" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="45" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="46"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="45" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="46"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="45" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="45" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="45" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+    </row>
+    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="45" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+    </row>
+    <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="45" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T12" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="48"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="47"/>
+      <c r="C16" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
create stage 12 + refactor code in file bloxorz_solver/function main
</commit_message>
<xml_diff>
--- a/stage_modeling.xlsx
+++ b/stage_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="stage_2" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="97">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -189,16 +189,19 @@
     <t xml:space="preserve">(1,-1)</t>
   </si>
   <si>
+    <t xml:space="preserve">(6,4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2,6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0,12)</t>
+  </si>
+  <si>
     <t xml:space="preserve">(6,2)</t>
   </si>
   <si>
-    <t xml:space="preserve">(6,4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2,6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0,12)</t>
+    <t xml:space="preserve">Bridge status</t>
   </si>
   <si>
     <t xml:space="preserve">2,4</t>
@@ -508,7 +511,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -685,23 +688,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -711,10 +698,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1124,39 +1107,39 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1184,17 +1167,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="49"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="6"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
       <c r="N5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1205,17 +1188,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
@@ -1224,17 +1207,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
@@ -1243,13 +1226,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1266,49 +1249,49 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="46"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1328,10 +1311,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1356,16 +1339,16 @@
         <v>6</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -1388,16 +1371,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1418,7 +1401,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>13</v>
@@ -1542,7 +1525,7 @@
       <c r="O1" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="P1" s="50" t="n">
+      <c r="P1" s="46" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1550,18 +1533,18 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -1570,10 +1553,10 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1597,13 +1580,13 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -1617,18 +1600,18 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -1636,61 +1619,61 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="46"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
       <c r="I7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
+        <v>66</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="46"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1699,20 +1682,20 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="46"/>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -1736,7 +1719,7 @@
         <v>1</v>
       </c>
       <c r="O10" s="3"/>
-      <c r="P10" s="46"/>
+      <c r="P10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1745,20 +1728,20 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
       <c r="M11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="46"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="V12" s="0" t="s">
@@ -1770,10 +1753,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1799,28 +1782,28 @@
         <v>6</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -1840,22 +1823,22 @@
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -1875,22 +1858,22 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -1910,16 +1893,16 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -1941,16 +1924,16 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1974,16 +1957,16 @@
         <v>30</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -2020,81 +2003,81 @@
   </sheetPr>
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="44" width="6.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="44" width="5.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="44" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45" t="n">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="n">
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="45" t="n">
+      <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="45" t="n">
+      <c r="E1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="45" t="n">
+      <c r="F1" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G1" s="45" t="n">
+      <c r="G1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H1" s="45" t="n">
+      <c r="H1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I1" s="45" t="n">
+      <c r="I1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J1" s="45" t="n">
+      <c r="J1" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K1" s="45" t="n">
+      <c r="K1" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="L1" s="45" t="n">
+      <c r="L1" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="M1" s="45" t="n">
+      <c r="M1" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="N1" s="45" t="n">
+      <c r="N1" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="n">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2122,84 +2105,84 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="n">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="n">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="n">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
         <v>3</v>
@@ -2213,235 +2196,235 @@
         <v>29</v>
       </c>
       <c r="L8" s="3"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="n">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-    </row>
-    <row r="10" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T10" s="51" t="s">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T10" s="44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="52" t="s">
+    <row r="11" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-    </row>
-    <row r="12" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="52" t="s">
+      <c r="C11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+    </row>
+    <row r="12" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="48" t="s">
+      <c r="C12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="D12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="E12" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-    </row>
-    <row r="13" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="52" t="s">
+      <c r="F12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+    </row>
+    <row r="13" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="48" t="s">
+      <c r="C13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" s="48" t="s">
+      <c r="E13" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-    </row>
-    <row r="14" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="52"/>
-      <c r="C14" s="48" t="s">
+      <c r="F13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+    </row>
+    <row r="14" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="47"/>
+      <c r="C14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+    </row>
+    <row r="15" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+    </row>
+    <row r="16" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="F16" s="44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-    </row>
-    <row r="15" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="48" t="s">
+      <c r="E17" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="48"/>
-    </row>
-    <row r="16" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="51" t="s">
+      <c r="E18" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="51" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="51" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="51" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" s="51" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="51" t="s">
-        <v>91</v>
+      <c r="E19" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -4097,8 +4080,8 @@
   </sheetPr>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4538,10 +4521,10 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Q6" activeCellId="0" sqref="Q6"/>
     </sheetView>
   </sheetViews>
@@ -4888,108 +4871,108 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="44" width="6.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="44" width="5.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="44" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45" t="n">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="n">
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="45" t="n">
+      <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="45" t="n">
+      <c r="E1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="45" t="n">
+      <c r="F1" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G1" s="45" t="n">
+      <c r="G1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H1" s="45" t="n">
+      <c r="H1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I1" s="45" t="n">
+      <c r="I1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J1" s="45" t="n">
+      <c r="J1" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K1" s="45" t="n">
+      <c r="K1" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="L1" s="45" t="n">
+      <c r="L1" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="M1" s="45" t="n">
+      <c r="M1" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="N1" s="45" t="n">
+      <c r="N1" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="n">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
         <v>0</v>
@@ -5002,62 +4985,62 @@
       <c r="N4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="D5" s="46"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="46"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="n">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="46"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="n">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="46"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="n">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="3"/>
@@ -5067,206 +5050,245 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="n">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45" t="n">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="45" t="n">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T12" s="44" t="s">
+      <c r="T12" s="0" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="48"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="47"/>
-      <c r="C16" s="48" t="s">
+      <c r="C17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="48"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="48"/>
-      <c r="T16" s="48"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="48"/>
-      <c r="S17" s="48"/>
-      <c r="T17" s="48"/>
+      <c r="D17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="44"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="44"/>
+      <c r="S18" s="44"/>
+      <c r="T18" s="44"/>
+      <c r="U18" s="44"/>
+      <c r="V18" s="44"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix bugs: consequence make state invalid
</commit_message>
<xml_diff>
--- a/stage_modeling.xlsx
+++ b/stage_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="stage_2" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="97">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -189,7 +189,7 @@
     <t xml:space="preserve">(1,-1)</t>
   </si>
   <si>
-    <t xml:space="preserve">(6,4)</t>
+    <t xml:space="preserve">(4,6)</t>
   </si>
   <si>
     <t xml:space="preserve">(2,6)</t>
@@ -784,7 +784,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="1" sqref="C21:J21 I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="P14" activeCellId="1" sqref="C21:J21 P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1468,10 +1468,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1984,6 +1984,35 @@
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="44" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2004,7 +2033,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="1" sqref="C21:J21 I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2446,7 +2475,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="1" sqref="C21:J21 H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2790,7 +2819,7 @@
   <dimension ref="A1:AG13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="C21:J21 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3260,7 +3289,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
+      <selection pane="topLeft" activeCell="R6" activeCellId="1" sqref="C21:J21 R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3540,7 +3569,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="C21:J21 A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3849,7 +3878,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="C21:J21 I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4081,7 +4110,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+      <selection pane="topLeft" activeCell="M11" activeCellId="1" sqref="C21:J21 M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4525,7 +4554,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q6" activeCellId="0" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="H8" activeCellId="1" sqref="C21:J21 H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4873,8 +4902,8 @@
   </sheetPr>
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="1" sqref="C21:J21 D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5013,7 +5042,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -5049,7 +5078,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>

</xml_diff>

<commit_message>
split function get_heuristic_rank + add some comments
</commit_message>
<xml_diff>
--- a/stage_modeling.xlsx
+++ b/stage_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="stage_1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,6 +23,7 @@
     <sheet name="stage_14" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="stage_15" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="stage_16" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="stage_20" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="98">
   <si>
     <t xml:space="preserve">S</t>
   </si>
@@ -523,7 +524,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -554,10 +555,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -724,6 +721,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -804,7 +809,7 @@
   <dimension ref="A1:AMJ13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="C13:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1077,7 +1082,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H8" activeCellId="1" sqref="C13:F22 H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1133,31 +1138,31 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1166,54 +1171,54 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="8"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="8"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="2"/>
@@ -1222,8 +1227,8 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1232,47 +1237,47 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1285,18 +1290,18 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="8"/>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S12" s="0" t="s">
@@ -1304,7 +1309,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1330,7 +1335,7 @@
       <c r="S13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1356,7 +1361,7 @@
       <c r="S14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1386,7 +1391,7 @@
       <c r="S15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="7"/>
@@ -1426,7 +1431,7 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="C13:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1482,18 +1487,18 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1502,16 +1507,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1520,11 +1525,11 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
         <v>9</v>
@@ -1534,58 +1539,58 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="11"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="8"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="8"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1601,11 +1606,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1619,51 +1624,51 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T12" s="0" t="s">
@@ -1671,7 +1676,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1700,7 +1705,7 @@
       <c r="V13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1731,7 +1736,7 @@
       <c r="V14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="7" t="s">
         <v>57</v>
       </c>
@@ -1760,7 +1765,7 @@
       <c r="V15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="7"/>
@@ -1785,7 +1790,7 @@
       <c r="V16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1814,7 +1819,7 @@
       <c r="V17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="5" t="n">
@@ -1860,8 +1865,8 @@
   </sheetPr>
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q10" activeCellId="1" sqref="C13:F22 Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1923,12 +1928,12 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="13"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -2001,9 +2006,9 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
         <v>1</v>
@@ -2024,7 +2029,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -2043,11 +2048,11 @@
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="3"/>
@@ -2062,12 +2067,12 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -2081,12 +2086,12 @@
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -2116,7 +2121,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7"/>
@@ -2141,7 +2146,7 @@
       <c r="V13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="7"/>
@@ -2166,7 +2171,7 @@
       <c r="V14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="7"/>
@@ -2191,7 +2196,7 @@
       <c r="V15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -2220,7 +2225,7 @@
       <c r="V16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="5"/>
@@ -2263,7 +2268,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
+      <selection pane="topLeft" activeCell="P14" activeCellId="1" sqref="C13:F22 P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2322,47 +2327,47 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
         <v>0</v>
@@ -2382,17 +2387,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="11"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2403,17 +2408,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
@@ -2422,17 +2427,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
@@ -2441,13 +2446,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -2464,49 +2469,49 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -2522,7 +2527,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -2550,7 +2555,7 @@
       <c r="U13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -2582,7 +2587,7 @@
       <c r="U14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -2614,7 +2619,7 @@
       <c r="U15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="7" t="s">
         <v>67</v>
       </c>
@@ -2644,7 +2649,7 @@
       <c r="U16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="7"/>
@@ -2686,7 +2691,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+      <selection pane="topLeft" activeCell="M11" activeCellId="1" sqref="C13:F22 M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2740,7 +2745,7 @@
       <c r="O1" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="P1" s="49" t="n">
+      <c r="P1" s="48" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2748,18 +2753,18 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -2768,18 +2773,18 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
       <c r="N3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2792,16 +2797,16 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -2815,18 +2820,18 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2834,61 +2839,61 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -2897,20 +2902,20 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="8"/>
+      <c r="P9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -2927,14 +2932,14 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="8"/>
+      <c r="P10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2943,20 +2948,20 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
       <c r="M11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="8"/>
+      <c r="P11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="V12" s="0" t="s">
@@ -2964,7 +2969,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -2993,7 +2998,7 @@
       <c r="V13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -3034,7 +3039,7 @@
       <c r="V14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -3071,7 +3076,7 @@
       <c r="V15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="7" t="s">
         <v>80</v>
       </c>
@@ -3106,7 +3111,7 @@
       <c r="V16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="7" t="s">
         <v>83</v>
       </c>
@@ -3137,7 +3142,7 @@
       <c r="V17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="7" t="s">
         <v>86</v>
       </c>
@@ -3168,7 +3173,7 @@
       <c r="V18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -3201,7 +3206,7 @@
       <c r="V19" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="5" t="n">
@@ -3248,7 +3253,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C13:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3304,18 +3309,18 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -3331,8 +3336,8 @@
       <c r="D3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3340,8 +3345,8 @@
         <v>9</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
         <v>1</v>
@@ -3352,18 +3357,18 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -3372,61 +3377,61 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
         <v>0</v>
@@ -3440,26 +3445,26 @@
         <v>34</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T10" s="5" t="s">
@@ -3687,6 +3692,437 @@
       <c r="F20" s="7" t="n">
         <v>0</v>
       </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:U22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="C13" activeCellId="0" sqref="C13:F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="17" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+    </row>
+    <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+    </row>
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U12" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+    </row>
+    <row r="15" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+    </row>
+    <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3707,7 +4143,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="1" sqref="C13:F22 I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3769,18 +4205,18 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -3793,18 +4229,18 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="P3" s="2"/>
@@ -3819,14 +4255,14 @@
         <v>10</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -3839,14 +4275,14 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -3856,19 +4292,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -3881,20 +4317,20 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -3905,7 +4341,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -3922,7 +4358,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -3971,7 +4407,7 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="C13:F22 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4034,13 +4470,13 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -4053,13 +4489,13 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -4137,11 +4573,11 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -4156,11 +4592,11 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -4178,10 +4614,10 @@
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="13"/>
+      <c r="O9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -4197,10 +4633,10 @@
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
     </row>
     <row r="11" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U11" s="5" t="s">
@@ -4335,7 +4771,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="1" sqref="C13:F22 H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4398,220 +4834,220 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="15"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="19" t="s">
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="15"/>
+      <c r="P3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="n">
+      <c r="A4" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="n">
+      <c r="A5" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="21"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="21"/>
-      <c r="S6" s="22"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="20"/>
+      <c r="S6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="21"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="14" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="n">
+      <c r="A9" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="26"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="32" t="s">
+      <c r="B10" s="29"/>
+      <c r="C10" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M12" s="37"/>
+      <c r="M12" s="36"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -4622,24 +5058,24 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38" t="s">
+      <c r="D14" s="37"/>
+      <c r="E14" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38" t="s">
+      <c r="F14" s="37"/>
+      <c r="G14" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="38"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -4679,15 +5115,15 @@
   <dimension ref="A1:AG13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <selection pane="topLeft" activeCell="K6" activeCellId="1" sqref="C13:F22 K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="2" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="39" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="18" style="39" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="38" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="18" style="38" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="8.45"/>
   </cols>
   <sheetData>
@@ -4738,136 +5174,136 @@
       <c r="P1" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
     </row>
     <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="41"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="42"/>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
-      <c r="AF2" s="42"/>
-      <c r="AG2" s="42"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="40"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="41"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="41"/>
-      <c r="R3" s="40"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="42"/>
-      <c r="AF3" s="42"/>
-      <c r="AG3" s="42"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="40"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
+      <c r="AG3" s="41"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="41"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="42"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="42"/>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="42"/>
-      <c r="AA4" s="42"/>
-      <c r="AB4" s="42"/>
-      <c r="AC4" s="42"/>
-      <c r="AD4" s="42"/>
-      <c r="AE4" s="42"/>
-      <c r="AF4" s="42"/>
-      <c r="AG4" s="42"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="40"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="41"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="2"/>
@@ -4875,252 +5311,252 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="43"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="42"/>
-      <c r="Z5" s="42"/>
-      <c r="AA5" s="42"/>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="42"/>
-      <c r="AD5" s="42"/>
-      <c r="AE5" s="42"/>
-      <c r="AF5" s="42"/>
-      <c r="AG5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="41"/>
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="41"/>
+      <c r="AD5" s="41"/>
+      <c r="AE5" s="41"/>
+      <c r="AF5" s="41"/>
+      <c r="AG5" s="41"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="43"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="42"/>
-      <c r="Z6" s="42"/>
-      <c r="AA6" s="42"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
-      <c r="AD6" s="42"/>
-      <c r="AE6" s="42"/>
-      <c r="AF6" s="42"/>
-      <c r="AG6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
+      <c r="AC6" s="41"/>
+      <c r="AD6" s="41"/>
+      <c r="AE6" s="41"/>
+      <c r="AF6" s="41"/>
+      <c r="AG6" s="41"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="43"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="42"/>
-      <c r="AB7" s="42"/>
-      <c r="AC7" s="42"/>
-      <c r="AD7" s="42"/>
-      <c r="AE7" s="42"/>
-      <c r="AF7" s="42"/>
-      <c r="AG7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
+      <c r="AE7" s="41"/>
+      <c r="AF7" s="41"/>
+      <c r="AG7" s="41"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="41"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="42"/>
-      <c r="Z8" s="42"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="42"/>
-      <c r="AC8" s="42"/>
-      <c r="AD8" s="42"/>
-      <c r="AE8" s="42"/>
-      <c r="AF8" s="42"/>
-      <c r="AG8" s="42"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="40"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
+      <c r="AC8" s="41"/>
+      <c r="AD8" s="41"/>
+      <c r="AE8" s="41"/>
+      <c r="AF8" s="41"/>
+      <c r="AG8" s="41"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="41"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="42"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="42"/>
-      <c r="V9" s="42"/>
-      <c r="W9" s="42"/>
-      <c r="X9" s="42"/>
-      <c r="Y9" s="42"/>
-      <c r="Z9" s="42"/>
-      <c r="AA9" s="42"/>
-      <c r="AB9" s="42"/>
-      <c r="AC9" s="42"/>
-      <c r="AD9" s="42"/>
-      <c r="AE9" s="42"/>
-      <c r="AF9" s="42"/>
-      <c r="AG9" s="42"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="40"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
+      <c r="AC9" s="41"/>
+      <c r="AD9" s="41"/>
+      <c r="AE9" s="41"/>
+      <c r="AF9" s="41"/>
+      <c r="AG9" s="41"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="41"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="42"/>
-      <c r="V10" s="42"/>
-      <c r="W10" s="42"/>
-      <c r="X10" s="42"/>
-      <c r="Y10" s="42"/>
-      <c r="Z10" s="42"/>
-      <c r="AA10" s="42"/>
-      <c r="AB10" s="42"/>
-      <c r="AC10" s="42"/>
-      <c r="AD10" s="42"/>
-      <c r="AE10" s="42"/>
-      <c r="AF10" s="42"/>
-      <c r="AG10" s="42"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="40"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="41"/>
+      <c r="AD10" s="41"/>
+      <c r="AE10" s="41"/>
+      <c r="AF10" s="41"/>
+      <c r="AG10" s="41"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="41"/>
-      <c r="R11" s="40"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="42"/>
-      <c r="W11" s="42"/>
-      <c r="X11" s="42"/>
-      <c r="Y11" s="42"/>
-      <c r="Z11" s="42"/>
-      <c r="AA11" s="42"/>
-      <c r="AB11" s="42"/>
-      <c r="AC11" s="42"/>
-      <c r="AD11" s="42"/>
-      <c r="AE11" s="42"/>
-      <c r="AF11" s="42"/>
-      <c r="AG11" s="42"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="40"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="41"/>
+      <c r="AD11" s="41"/>
+      <c r="AE11" s="41"/>
+      <c r="AF11" s="41"/>
+      <c r="AG11" s="41"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -5149,7 +5585,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C13:F22 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5211,41 +5647,41 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -5254,14 +5690,14 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -5272,7 +5708,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2"/>
@@ -5282,11 +5718,11 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="P5" s="2"/>
@@ -5298,17 +5734,17 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -5320,15 +5756,15 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -5337,44 +5773,44 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -5385,7 +5821,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -5396,7 +5832,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -5429,7 +5865,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="C13:F22 A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5491,61 +5927,61 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="46"/>
+      <c r="L3" s="45"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -5557,9 +5993,9 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -5572,7 +6008,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2"/>
@@ -5581,14 +6017,14 @@
         <v>34</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="P6" s="2"/>
@@ -5603,9 +6039,9 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -5617,64 +6053,64 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -5685,7 +6121,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7"/>
@@ -5694,7 +6130,7 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="7"/>
@@ -5703,7 +6139,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -5738,7 +6174,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="C13:F22 I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5804,13 +6240,13 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -5821,20 +6257,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="45"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="46"/>
+      <c r="N3" s="45"/>
       <c r="O3" s="2" t="s">
         <v>34</v>
       </c>
@@ -5864,41 +6300,41 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="P5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="V7" s="0" t="s">
@@ -5906,7 +6342,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -5917,7 +6353,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="7"/>
@@ -5926,7 +6362,7 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="7"/>
@@ -5935,7 +6371,7 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -5970,7 +6406,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+      <selection pane="topLeft" activeCell="M11" activeCellId="1" sqref="C13:F22 M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6032,11 +6468,11 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -6049,22 +6485,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="45" t="s">
         <v>0</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="46" t="s">
+      <c r="N3" s="45" t="s">
         <v>34</v>
       </c>
       <c r="O3" s="2"/>
@@ -6076,145 +6512,145 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="8"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="23"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="8"/>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="8"/>
+      <c r="O7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="8"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="8"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="8"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -6222,7 +6658,7 @@
         <v>9</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="8"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U12" s="0" t="s">
@@ -6230,7 +6666,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -6258,7 +6694,7 @@
       <c r="U13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -6294,7 +6730,7 @@
       <c r="U14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -6326,7 +6762,7 @@
       <c r="U15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="7" t="s">
         <v>48</v>
       </c>
@@ -6360,7 +6796,7 @@
       <c r="U16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="7" t="s">

</xml_diff>